<commit_message>
Budget US sheet Update
</commit_message>
<xml_diff>
--- a/budget-web-tests/testData/Budget_Anonymous_US.xlsx
+++ b/budget-web-tests/testData/Budget_Anonymous_US.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/StatusNeo/Desktop/Budget_Payless 27 Apr/ecom-us-web/budget-web-tests/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886F84E7-DD3C-0541-B407-31842876EA82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA96362C-B2F1-5145-AF8C-942B08853EBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,7 +493,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -517,9 +517,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
@@ -1029,10 +1026,10 @@
       <c r="BL1" t="s">
         <v>120</v>
       </c>
-      <c r="BM1" s="11" t="s">
+      <c r="BM1" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="BN1" s="11" t="s">
+      <c r="BN1" s="10" t="s">
         <v>122</v>
       </c>
       <c r="BO1" s="3" t="s">
@@ -1044,7 +1041,7 @@
       <c r="BQ1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="BR1" s="13" t="s">
+      <c r="BR1" s="12" t="s">
         <v>119</v>
       </c>
     </row>
@@ -1238,13 +1235,13 @@
       <c r="BK2" t="s">
         <v>66</v>
       </c>
-      <c r="BL2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN2" s="12" t="s">
+      <c r="BL2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM2" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN2" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO2" t="s">
@@ -1450,13 +1447,13 @@
       <c r="BK3" t="s">
         <v>66</v>
       </c>
-      <c r="BL3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM3" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN3" s="12" t="s">
+      <c r="BL3" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM3" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN3" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO3" t="s">
@@ -1662,13 +1659,13 @@
       <c r="BK4" t="s">
         <v>66</v>
       </c>
-      <c r="BL4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN4" s="12" t="s">
+      <c r="BL4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM4" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN4" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO4" t="s">
@@ -1874,13 +1871,13 @@
       <c r="BK5" t="s">
         <v>66</v>
       </c>
-      <c r="BL5" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM5" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN5" s="12" t="s">
+      <c r="BL5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN5" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO5" t="s">
@@ -2086,13 +2083,13 @@
       <c r="BK6" t="s">
         <v>66</v>
       </c>
-      <c r="BL6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM6" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN6" s="12" t="s">
+      <c r="BL6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN6" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO6" t="s">
@@ -2298,13 +2295,13 @@
       <c r="BK7" t="s">
         <v>66</v>
       </c>
-      <c r="BL7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM7" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN7" s="12" t="s">
+      <c r="BL7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM7" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN7" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO7" t="s">
@@ -2510,13 +2507,13 @@
       <c r="BK8" t="s">
         <v>66</v>
       </c>
-      <c r="BL8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM8" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN8" s="12" t="s">
+      <c r="BL8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN8" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO8" t="s">
@@ -2722,13 +2719,13 @@
       <c r="BK9" t="s">
         <v>66</v>
       </c>
-      <c r="BL9" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM9" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN9" s="12" t="s">
+      <c r="BL9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM9" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN9" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO9" t="s">
@@ -2934,13 +2931,13 @@
       <c r="BK10" t="s">
         <v>66</v>
       </c>
-      <c r="BL10" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM10" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN10" s="12" t="s">
+      <c r="BL10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM10" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN10" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO10" t="s">
@@ -2973,19 +2970,19 @@
         <v>66</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="G11" t="s">
         <v>66</v>
       </c>
       <c r="H11" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="I11" t="s">
         <v>66</v>
       </c>
       <c r="J11" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="K11" t="s">
         <v>66</v>
@@ -3146,13 +3143,13 @@
       <c r="BK11" t="s">
         <v>66</v>
       </c>
-      <c r="BL11" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM11" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN11" s="12" t="s">
+      <c r="BL11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN11" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO11" t="s">
@@ -3265,7 +3262,7 @@
       <c r="AF12" t="s">
         <v>100</v>
       </c>
-      <c r="AG12" s="9">
+      <c r="AG12" s="6">
         <v>112000000000</v>
       </c>
       <c r="AH12" t="s">
@@ -3358,13 +3355,13 @@
       <c r="BK12" t="s">
         <v>66</v>
       </c>
-      <c r="BL12" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM12" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN12" s="12" t="s">
+      <c r="BL12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM12" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN12" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO12" t="s">
@@ -3570,13 +3567,13 @@
       <c r="BK13" t="s">
         <v>66</v>
       </c>
-      <c r="BL13" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM13" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN13" s="12" t="s">
+      <c r="BL13" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM13" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN13" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO13" t="s">
@@ -3614,7 +3611,7 @@
       <c r="G14" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="15" t="s">
+      <c r="H14" s="14" t="s">
         <v>104</v>
       </c>
       <c r="I14" t="s">
@@ -3782,13 +3779,13 @@
       <c r="BK14" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="BL14" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM14" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="BN14" s="12" t="s">
+      <c r="BL14" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM14" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="BN14" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO14" t="s">
@@ -3826,13 +3823,13 @@
       <c r="G15" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="15" t="s">
+      <c r="H15" s="14" t="s">
         <v>104</v>
       </c>
       <c r="I15" t="s">
         <v>66</v>
       </c>
-      <c r="J15" s="15" t="s">
+      <c r="J15" s="14" t="s">
         <v>127</v>
       </c>
       <c r="K15" t="s">
@@ -3991,13 +3988,13 @@
       <c r="BK15" t="s">
         <v>66</v>
       </c>
-      <c r="BL15" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM15" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN15" s="12" t="s">
+      <c r="BL15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN15" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO15" t="s">
@@ -4173,7 +4170,7 @@
       <c r="BA16" t="s">
         <v>66</v>
       </c>
-      <c r="BB16" s="10" t="s">
+      <c r="BB16" s="9" t="s">
         <v>109</v>
       </c>
       <c r="BC16">
@@ -4203,13 +4200,13 @@
       <c r="BK16" t="s">
         <v>66</v>
       </c>
-      <c r="BL16" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM16" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN16" s="12" t="s">
+      <c r="BL16" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM16" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN16" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO16" t="s">
@@ -4415,13 +4412,13 @@
       <c r="BK17" t="s">
         <v>66</v>
       </c>
-      <c r="BL17" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM17" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN17" s="12" t="s">
+      <c r="BL17" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM17" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN17" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO17" t="s">
@@ -4627,13 +4624,13 @@
       <c r="BK18" t="s">
         <v>66</v>
       </c>
-      <c r="BL18" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM18" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN18" s="12" t="s">
+      <c r="BL18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM18" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN18" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO18" s="3" t="s">
@@ -4839,22 +4836,22 @@
       <c r="BK19" t="s">
         <v>66</v>
       </c>
-      <c r="BL19" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM19" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN19" s="12" t="s">
+      <c r="BL19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM19" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN19" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BO19" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="BP19" s="14" t="s">
+      <c r="BP19" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="BQ19" s="14" t="s">
+      <c r="BQ19" s="13" t="s">
         <v>125</v>
       </c>
       <c r="BR19" t="s">
@@ -5051,16 +5048,16 @@
       <c r="BK20" t="s">
         <v>66</v>
       </c>
-      <c r="BL20" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM20" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN20" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BO20" s="12" t="s">
+      <c r="BL20" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM20" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN20" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BO20" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BP20" t="s">
@@ -5263,16 +5260,16 @@
       <c r="BK21" t="s">
         <v>66</v>
       </c>
-      <c r="BL21" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BM21" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BN21" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="BO21" s="12" t="s">
+      <c r="BL21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BM21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BN21" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="BO21" s="11" t="s">
         <v>66</v>
       </c>
       <c r="BP21" t="s">

</xml_diff>